<commit_message>
With arab cities as well
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -2549,7 +2549,9 @@
       <c r="D17" s="14">
         <v>14099</v>
       </c>
-      <c r="E17" s="13"/>
+      <c r="E17" s="14">
+        <v>0</v>
+      </c>
       <c r="F17" s="14">
         <v>6831.893346379650</v>
       </c>
@@ -2594,7 +2596,9 @@
       <c r="D18" s="14">
         <v>17171</v>
       </c>
-      <c r="E18" s="13"/>
+      <c r="E18" s="14">
+        <v>0</v>
+      </c>
       <c r="F18" s="17">
         <v>7154.488748187280</v>
       </c>
@@ -2639,7 +2643,9 @@
       <c r="D19" s="14">
         <v>17171</v>
       </c>
-      <c r="E19" s="13"/>
+      <c r="E19" s="14">
+        <v>0</v>
+      </c>
       <c r="F19" s="17">
         <v>7154.488748187280</v>
       </c>
@@ -2864,7 +2870,9 @@
       <c r="D24" s="14">
         <v>21163</v>
       </c>
-      <c r="E24" s="13"/>
+      <c r="E24" s="14">
+        <v>0</v>
+      </c>
       <c r="F24" s="15">
         <v>6229.070961768870</v>
       </c>
@@ -2909,7 +2917,9 @@
       <c r="D25" s="14">
         <v>21163</v>
       </c>
-      <c r="E25" s="13"/>
+      <c r="E25" s="14">
+        <v>0</v>
+      </c>
       <c r="F25" s="15">
         <v>6229.070961768870</v>
       </c>
@@ -3040,7 +3050,9 @@
       <c r="D28" s="14">
         <v>15455</v>
       </c>
-      <c r="E28" s="13"/>
+      <c r="E28" s="14">
+        <v>0</v>
+      </c>
       <c r="F28" s="17">
         <v>6120.264638811240</v>
       </c>
@@ -3085,7 +3097,9 @@
       <c r="D29" s="14">
         <v>15455</v>
       </c>
-      <c r="E29" s="13"/>
+      <c r="E29" s="14">
+        <v>0</v>
+      </c>
       <c r="F29" s="17">
         <v>6120.264638811240</v>
       </c>
@@ -3130,7 +3144,9 @@
       <c r="D30" s="14">
         <v>22957</v>
       </c>
-      <c r="E30" s="13"/>
+      <c r="E30" s="14">
+        <v>0</v>
+      </c>
       <c r="F30" s="15">
         <v>6918.322488999760</v>
       </c>
@@ -3175,7 +3191,9 @@
       <c r="D31" s="14">
         <v>22957</v>
       </c>
-      <c r="E31" s="13"/>
+      <c r="E31" s="14">
+        <v>0</v>
+      </c>
       <c r="F31" s="15">
         <v>6918.322488999760</v>
       </c>
@@ -3220,7 +3238,9 @@
       <c r="D32" s="14">
         <v>34392</v>
       </c>
-      <c r="E32" s="13"/>
+      <c r="E32" s="14">
+        <v>0</v>
+      </c>
       <c r="F32" s="15">
         <v>6089.859782711830</v>
       </c>
@@ -3265,7 +3285,9 @@
       <c r="D33" s="14">
         <v>34392</v>
       </c>
-      <c r="E33" s="13"/>
+      <c r="E33" s="14">
+        <v>0</v>
+      </c>
       <c r="F33" s="15">
         <v>6089.859782711830</v>
       </c>
@@ -3310,7 +3332,9 @@
       <c r="D34" s="14">
         <v>31702</v>
       </c>
-      <c r="E34" s="13"/>
+      <c r="E34" s="14">
+        <v>0</v>
+      </c>
       <c r="F34" s="15">
         <v>6617.165072760010</v>
       </c>
@@ -3355,7 +3379,9 @@
       <c r="D35" s="14">
         <v>31702</v>
       </c>
-      <c r="E35" s="13"/>
+      <c r="E35" s="14">
+        <v>0</v>
+      </c>
       <c r="F35" s="15">
         <v>6617.165072760010</v>
       </c>
@@ -3494,7 +3520,9 @@
       <c r="D38" s="14">
         <v>25833</v>
       </c>
-      <c r="E38" s="13"/>
+      <c r="E38" s="14">
+        <v>0</v>
+      </c>
       <c r="F38" s="15">
         <v>6592.854868240930</v>
       </c>
@@ -3539,7 +3567,9 @@
       <c r="D39" s="14">
         <v>25833</v>
       </c>
-      <c r="E39" s="13"/>
+      <c r="E39" s="14">
+        <v>0</v>
+      </c>
       <c r="F39" s="15">
         <v>6592.854868240930</v>
       </c>
@@ -3772,7 +3802,9 @@
       <c r="D44" s="14">
         <v>13305</v>
       </c>
-      <c r="E44" s="13"/>
+      <c r="E44" s="14">
+        <v>0</v>
+      </c>
       <c r="F44" s="15">
         <v>6609.757156741470</v>
       </c>
@@ -3997,7 +4029,9 @@
       <c r="D49" s="14">
         <v>42137</v>
       </c>
-      <c r="E49" s="13"/>
+      <c r="E49" s="14">
+        <v>0</v>
+      </c>
       <c r="F49" s="15">
         <v>6911.339523967920</v>
       </c>
@@ -4042,7 +4076,9 @@
       <c r="D50" s="14">
         <v>42137</v>
       </c>
-      <c r="E50" s="13"/>
+      <c r="E50" s="14">
+        <v>0</v>
+      </c>
       <c r="F50" s="15">
         <v>6911.339523967920</v>
       </c>
@@ -4721,7 +4757,9 @@
       <c r="D65" s="14">
         <v>22751</v>
       </c>
-      <c r="E65" s="13"/>
+      <c r="E65" s="14">
+        <v>0</v>
+      </c>
       <c r="F65" s="15">
         <v>5848.884750352820</v>
       </c>
@@ -4766,7 +4804,9 @@
       <c r="D66" s="14">
         <v>22751</v>
       </c>
-      <c r="E66" s="13"/>
+      <c r="E66" s="14">
+        <v>0</v>
+      </c>
       <c r="F66" s="15">
         <v>5848.884750352820</v>
       </c>
@@ -4999,7 +5039,9 @@
       <c r="D71" s="14">
         <v>19001</v>
       </c>
-      <c r="E71" s="13"/>
+      <c r="E71" s="14">
+        <v>0</v>
+      </c>
       <c r="F71" s="15">
         <v>6365.206813843680</v>
       </c>
@@ -5044,7 +5086,9 @@
       <c r="D72" s="14">
         <v>77445</v>
       </c>
-      <c r="E72" s="13"/>
+      <c r="E72" s="14">
+        <v>0</v>
+      </c>
       <c r="F72" s="15">
         <v>6787.750989201430</v>
       </c>
@@ -5089,7 +5133,9 @@
       <c r="D73" s="14">
         <v>77445</v>
       </c>
-      <c r="E73" s="13"/>
+      <c r="E73" s="14">
+        <v>0</v>
+      </c>
       <c r="F73" s="15">
         <v>6787.750989201430</v>
       </c>
@@ -5134,7 +5180,9 @@
       <c r="D74" s="14">
         <v>17653</v>
       </c>
-      <c r="E74" s="13"/>
+      <c r="E74" s="14">
+        <v>0</v>
+      </c>
       <c r="F74" s="14">
         <v>8024.372532413220</v>
       </c>
@@ -5179,7 +5227,9 @@
       <c r="D75" s="14">
         <v>17653</v>
       </c>
-      <c r="E75" s="13"/>
+      <c r="E75" s="14">
+        <v>0</v>
+      </c>
       <c r="F75" s="14">
         <v>8024.372532413220</v>
       </c>
@@ -5224,7 +5274,9 @@
       <c r="D76" s="14">
         <v>19151</v>
       </c>
-      <c r="E76" s="13"/>
+      <c r="E76" s="14">
+        <v>0</v>
+      </c>
       <c r="F76" s="15">
         <v>6351.4990304016</v>
       </c>
@@ -5903,7 +5955,9 @@
       <c r="D91" s="14">
         <v>56109</v>
       </c>
-      <c r="E91" s="13"/>
+      <c r="E91" s="14">
+        <v>0</v>
+      </c>
       <c r="F91" s="15">
         <v>5851.761229429630</v>
       </c>
@@ -5948,7 +6002,9 @@
       <c r="D92" s="14">
         <v>56109</v>
       </c>
-      <c r="E92" s="13"/>
+      <c r="E92" s="14">
+        <v>0</v>
+      </c>
       <c r="F92" s="15">
         <v>5851.761229429630</v>
       </c>
@@ -6267,7 +6323,9 @@
       <c r="D99" s="14">
         <v>19018</v>
       </c>
-      <c r="E99" s="13"/>
+      <c r="E99" s="14">
+        <v>0</v>
+      </c>
       <c r="F99" s="14">
         <v>7492.605373904270</v>
       </c>
@@ -6312,7 +6370,9 @@
       <c r="D100" s="14">
         <v>19018</v>
       </c>
-      <c r="E100" s="13"/>
+      <c r="E100" s="14">
+        <v>0</v>
+      </c>
       <c r="F100" s="14">
         <v>7492.605373904270</v>
       </c>
@@ -6451,7 +6511,9 @@
       <c r="D103" s="14">
         <v>25245</v>
       </c>
-      <c r="E103" s="13"/>
+      <c r="E103" s="14">
+        <v>0</v>
+      </c>
       <c r="F103" s="15">
         <v>6865.307956308940</v>
       </c>
@@ -6496,7 +6558,9 @@
       <c r="D104" s="14">
         <v>25245</v>
       </c>
-      <c r="E104" s="13"/>
+      <c r="E104" s="14">
+        <v>0</v>
+      </c>
       <c r="F104" s="15">
         <v>6865.307956308940</v>
       </c>
@@ -6729,7 +6793,9 @@
       <c r="D109" s="14">
         <v>29950</v>
       </c>
-      <c r="E109" s="13"/>
+      <c r="E109" s="14">
+        <v>0</v>
+      </c>
       <c r="F109" s="15">
         <v>6983.892909630370</v>
       </c>
@@ -6774,7 +6840,9 @@
       <c r="D110" s="14">
         <v>29950</v>
       </c>
-      <c r="E110" s="13"/>
+      <c r="E110" s="14">
+        <v>0</v>
+      </c>
       <c r="F110" s="15">
         <v>6983.892909630370</v>
       </c>
@@ -7179,7 +7247,9 @@
       <c r="D119" s="14">
         <v>23143</v>
       </c>
-      <c r="E119" s="13"/>
+      <c r="E119" s="14">
+        <v>0</v>
+      </c>
       <c r="F119" s="15">
         <v>6778.793916957030</v>
       </c>
@@ -7224,7 +7294,9 @@
       <c r="D120" s="14">
         <v>23143</v>
       </c>
-      <c r="E120" s="13"/>
+      <c r="E120" s="14">
+        <v>0</v>
+      </c>
       <c r="F120" s="15">
         <v>6778.793916957030</v>
       </c>
@@ -7543,7 +7615,9 @@
       <c r="D127" s="14">
         <v>43957</v>
       </c>
-      <c r="E127" s="13"/>
+      <c r="E127" s="14">
+        <v>0</v>
+      </c>
       <c r="F127" s="15">
         <v>6438.2376713218</v>
       </c>
@@ -7682,7 +7756,9 @@
       <c r="D130" s="14">
         <v>26552</v>
       </c>
-      <c r="E130" s="13"/>
+      <c r="E130" s="14">
+        <v>0</v>
+      </c>
       <c r="F130" s="15">
         <v>6987.973112778540</v>
       </c>
@@ -7727,7 +7803,9 @@
       <c r="D131" s="14">
         <v>26552</v>
       </c>
-      <c r="E131" s="13"/>
+      <c r="E131" s="14">
+        <v>0</v>
+      </c>
       <c r="F131" s="15">
         <v>6987.973112778540</v>
       </c>
@@ -8465,7 +8543,9 @@
       <c r="D147" s="14">
         <v>23823</v>
       </c>
-      <c r="E147" s="13"/>
+      <c r="E147" s="14">
+        <v>0</v>
+      </c>
       <c r="F147" s="15">
         <v>6425.510896303230</v>
       </c>
@@ -8510,7 +8590,9 @@
       <c r="D148" s="14">
         <v>23823</v>
       </c>
-      <c r="E148" s="13"/>
+      <c r="E148" s="14">
+        <v>0</v>
+      </c>
       <c r="F148" s="15">
         <v>6425.510896303230</v>
       </c>
@@ -12000,7 +12082,9 @@
       <c r="D224" s="14">
         <v>7698</v>
       </c>
-      <c r="E224" s="13"/>
+      <c r="E224" s="14">
+        <v>0</v>
+      </c>
       <c r="F224" s="15">
         <v>7271.2774521591</v>
       </c>
@@ -12045,7 +12129,9 @@
       <c r="D225" s="14">
         <v>7698</v>
       </c>
-      <c r="E225" s="13"/>
+      <c r="E225" s="14">
+        <v>0</v>
+      </c>
       <c r="F225" s="15">
         <v>7271.2774521591</v>
       </c>
@@ -13452,7 +13538,9 @@
       <c r="D256" s="14">
         <v>71437</v>
       </c>
-      <c r="E256" s="13"/>
+      <c r="E256" s="14">
+        <v>0</v>
+      </c>
       <c r="F256" s="15">
         <v>5719.1840351555</v>
       </c>
@@ -13497,7 +13585,9 @@
       <c r="D257" s="14">
         <v>71437</v>
       </c>
-      <c r="E257" s="13"/>
+      <c r="E257" s="14">
+        <v>0</v>
+      </c>
       <c r="F257" s="15">
         <v>5719.1840351555</v>
       </c>

</xml_diff>